<commit_message>
default gpt-4o, workng on chatgpt ner block
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_en/lab_app_nlu_knowledge_en.xlsx
+++ b/sample_apps/lab_app_en/lab_app_nlu_knowledge_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\lab_app_en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3F5FD8-43F7-4FFF-93BF-DF7C891F4DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99828DF8-FBA7-4EB5-8BF4-32A2400165D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="33750" yWindow="2850" windowWidth="21600" windowHeight="11055" activeTab="1" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="utterances" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>type</t>
     <phoneticPr fontId="1"/>
@@ -194,10 +194,6 @@
   </si>
   <si>
     <t>Vegetable Sandwiches, vegetable</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>cd s</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -605,15 +601,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8F96FF-CF47-4A99-83E7-8D5E860D6DFF}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -663,7 +659,7 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -677,7 +673,7 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -691,7 +687,7 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -738,14 +734,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E27BD90-5E4C-4A7C-B9E8-ABC211947ECB}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -768,7 +764,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>

</xml_diff>